<commit_message>
HEEDLS-810 - add PRN to download and tackle review comments
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Data.Tests/TestData/AllDelegatesExportTest.xlsx
+++ b/DigitalLearningSolutions.Data.Tests/TestData/AllDelegatesExportTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danblo\source\repos\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63D967-F756-4413-8DE4-B4043459680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22016021-6E15-4F48-B05A-84FD701EF228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Last name</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>TT95</t>
+  </si>
+  <si>
+    <t>Professional Registration Number</t>
+  </si>
+  <si>
+    <t>Not professionally registered</t>
+  </si>
+  <si>
+    <t>Not yet provided</t>
+  </si>
+  <si>
+    <t>MammalHands</t>
   </si>
 </sst>
 </file>
@@ -184,13 +196,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P4" totalsRowShown="0">
-  <autoFilter ref="A1:P4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q4" totalsRowShown="0">
+  <autoFilter ref="A1:Q4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Last name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="First name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ID"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email"/>
+    <tableColumn id="17" xr3:uid="{E0430E23-9661-4EE9-BDD1-546219A589D2}" name="Professional Registration Number"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Alias"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Job group"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Registered" dataDxfId="0"/>
@@ -493,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -504,21 +517,21 @@
     <col min="1" max="1" width="13.26171875" customWidth="1"/>
     <col min="2" max="2" width="13.5234375" customWidth="1"/>
     <col min="3" max="3" width="7.578125" customWidth="1"/>
-    <col min="4" max="4" width="30.15625" customWidth="1"/>
-    <col min="5" max="5" width="8.5234375" customWidth="1"/>
-    <col min="6" max="6" width="36.7890625" customWidth="1"/>
-    <col min="7" max="7" width="19.89453125" customWidth="1"/>
-    <col min="8" max="8" width="42" customWidth="1"/>
-    <col min="9" max="9" width="12.20703125" customWidth="1"/>
-    <col min="10" max="10" width="27.578125" customWidth="1"/>
-    <col min="11" max="12" width="28.3671875" customWidth="1"/>
-    <col min="13" max="13" width="15.734375" customWidth="1"/>
-    <col min="14" max="14" width="9.83984375" customWidth="1"/>
-    <col min="15" max="15" width="12.89453125" customWidth="1"/>
-    <col min="16" max="16" width="11.734375" customWidth="1"/>
+    <col min="4" max="5" width="30.15625" customWidth="1"/>
+    <col min="6" max="6" width="8.5234375" customWidth="1"/>
+    <col min="7" max="7" width="36.7890625" customWidth="1"/>
+    <col min="8" max="8" width="19.89453125" customWidth="1"/>
+    <col min="9" max="9" width="42" customWidth="1"/>
+    <col min="10" max="10" width="12.20703125" customWidth="1"/>
+    <col min="11" max="11" width="27.578125" customWidth="1"/>
+    <col min="12" max="13" width="28.3671875" customWidth="1"/>
+    <col min="14" max="14" width="15.734375" customWidth="1"/>
+    <col min="15" max="15" width="9.83984375" customWidth="1"/>
+    <col min="16" max="16" width="12.89453125" customWidth="1"/>
+    <col min="17" max="17" width="11.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,43 +545,46 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -581,15 +597,15 @@
       <c r="D2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>44620</v>
       </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
@@ -597,10 +613,13 @@
         <v>1</v>
       </c>
       <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -610,32 +629,35 @@
       <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>44651</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="b">
+      <c r="N3" t="b">
         <v>0</v>
       </c>
-      <c r="N3" t="b">
-        <v>1</v>
-      </c>
       <c r="O3" t="b">
         <v>1</v>
       </c>
       <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -645,21 +667,21 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>36526</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
       <c r="N4" t="b">
         <v>1</v>
       </c>
@@ -669,15 +691,18 @@
       <c r="P4" t="b">
         <v>1</v>
       </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G5" s="1"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G6" s="1"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G7" s="1"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
HEEDLS-980 Remove Alias from delegate spreadsheet journeys
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Data.Tests/TestData/AllDelegatesExportTest.xlsx
+++ b/DigitalLearningSolutions.Data.Tests/TestData/AllDelegatesExportTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danblo\source\repos\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejac\Git\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22016021-6E15-4F48-B05A-84FD701EF228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA97731-D4B6-4CCE-B37C-F56FF1C9E76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllDelegates" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Last name</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>Alias</t>
   </si>
   <si>
     <t>Job group</t>
@@ -180,7 +177,15 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -196,15 +201,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q4" totalsRowShown="0">
-  <autoFilter ref="A1:Q4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P4" totalsRowShown="0">
+  <autoFilter ref="A1:P4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Last name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="First name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ID"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email"/>
     <tableColumn id="17" xr3:uid="{E0430E23-9661-4EE9-BDD1-546219A589D2}" name="Professional Registration Number"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Alias"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Job group"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Registered" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Role type"/>
@@ -506,32 +510,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26171875" customWidth="1"/>
-    <col min="2" max="2" width="13.5234375" customWidth="1"/>
-    <col min="3" max="3" width="7.578125" customWidth="1"/>
-    <col min="4" max="5" width="30.15625" customWidth="1"/>
-    <col min="6" max="6" width="8.5234375" customWidth="1"/>
-    <col min="7" max="7" width="36.7890625" customWidth="1"/>
-    <col min="8" max="8" width="19.89453125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="9" width="42" customWidth="1"/>
-    <col min="10" max="10" width="12.20703125" customWidth="1"/>
-    <col min="11" max="11" width="27.578125" customWidth="1"/>
-    <col min="12" max="13" width="28.3671875" customWidth="1"/>
-    <col min="14" max="14" width="15.734375" customWidth="1"/>
-    <col min="15" max="15" width="9.83984375" customWidth="1"/>
-    <col min="16" max="16" width="12.89453125" customWidth="1"/>
-    <col min="17" max="17" width="11.734375" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="12" max="13" width="28.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -563,13 +566,13 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
         <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -580,128 +583,125 @@
       <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="4">
+        <v>44620</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="4">
+        <v>44651</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="4">
-        <v>44620</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
+      <c r="G4" s="4">
+        <v>36526</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="4">
-        <v>44651</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4">
-        <v>36526</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H7" s="1"/>
     </row>
   </sheetData>

</xml_diff>